<commit_message>
PCB update: - double /CS.i pad - color carrier generate inside CPLD (trace removed) - replace resistor arrays by simple components - add footprint for resistor from SNES mainboard to have resistor not loosely connected
</commit_message>
<xml_diff>
--- a/MultiRegion_with_DeJitter_QID/BOM.xlsx
+++ b/MultiRegion_with_DeJitter_QID/BOM.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="d:\Users\Peter\Documents\Workspaces\Git\SNES-AddOn-PCBs\MultiRegion_with_DeJitter_QID\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UserData\Bartmann\Workspaces\Git\Eigenes\SNES-AddOn-PCBs\MultiRegion_with_DeJitter_QID\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1E3B7CF-86C9-4D42-9BEF-544BFD173A3A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="30930" windowHeight="16890"/>
   </bookViews>
   <sheets>
-    <sheet name="V20190509" sheetId="3" r:id="rId1"/>
+    <sheet name="SMR20190813" sheetId="4" r:id="rId1"/>
+    <sheet name="SMR20190509" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029" refMode="R1C1" concurrentCalc="0"/>
+  <calcPr calcId="162913" refMode="R1C1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="330"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="119">
   <si>
     <t>Designator</t>
   </si>
@@ -366,13 +366,37 @@
   </si>
   <si>
     <t>(1uF cap 0603)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RC0603FR-0739RL </t>
+  </si>
+  <si>
+    <t>R53,R54,R61</t>
+  </si>
+  <si>
+    <t>R62</t>
+  </si>
+  <si>
+    <t>Resistor / Jumper</t>
+  </si>
+  <si>
+    <t>resistor taken from SNES mainboard / jumper closed, if CClk.o directly connected to SNES</t>
+  </si>
+  <si>
+    <t>Version:</t>
+  </si>
+  <si>
+    <t>SMR20190509</t>
+  </si>
+  <si>
+    <t>SMR20190813</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -511,6 +535,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -858,7 +890,7 @@
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -879,14 +911,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1208,182 +1241,136 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K41"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.44140625" customWidth="1"/>
-    <col min="5" max="5" width="23.44140625" customWidth="1"/>
-    <col min="8" max="8" width="59.88671875" customWidth="1"/>
-    <col min="9" max="9" width="11.33203125" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" customWidth="1"/>
+    <col min="5" max="5" width="23.42578125" customWidth="1"/>
+    <col min="8" max="8" width="59.85546875" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="18" t="s">
+        <v>116</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="13">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C5" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D5" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F5" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="H5" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="I5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="J5" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="K3" s="5" t="s">
+      <c r="K5" s="5" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" t="s">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
         <v>32</v>
       </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4">
-        <f>C4*D$1</f>
-        <v>3</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <f>C6*D$3</f>
+        <v>3</v>
+      </c>
+      <c r="E6" t="s">
         <v>33</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G6" t="s">
         <v>34</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H6" t="s">
         <v>36</v>
-      </c>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5">
-        <f t="shared" ref="D5:D19" si="0">C5*D$1</f>
-        <v>3</v>
-      </c>
-      <c r="E5" t="s">
-        <v>33</v>
-      </c>
-      <c r="G5" t="s">
-        <v>34</v>
-      </c>
-      <c r="H5" t="s">
-        <v>38</v>
-      </c>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="D6">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="E6" t="s">
-        <v>40</v>
-      </c>
-      <c r="G6" t="s">
-        <v>41</v>
-      </c>
-      <c r="H6" t="s">
-        <v>42</v>
       </c>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
       <c r="K6" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>90</v>
+        <v>35</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
       <c r="D7">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="D7:D21" si="0">C7*D$3</f>
         <v>3</v>
       </c>
       <c r="E7" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="G7" t="s">
-        <v>94</v>
+        <v>34</v>
+      </c>
+      <c r="H7" t="s">
+        <v>38</v>
       </c>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K7" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -1393,26 +1380,26 @@
         <v>3</v>
       </c>
       <c r="E8" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="G8" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="H8" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
-      <c r="K8" s="15" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K8" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>76</v>
+        <v>90</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -1422,20 +1409,20 @@
         <v>3</v>
       </c>
       <c r="E9" t="s">
-        <v>77</v>
+        <v>47</v>
       </c>
       <c r="G9" t="s">
-        <v>78</v>
+        <v>94</v>
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -1445,20 +1432,26 @@
         <v>3</v>
       </c>
       <c r="E10" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="G10" t="s">
-        <v>19</v>
+        <v>45</v>
+      </c>
+      <c r="H10" t="s">
+        <v>46</v>
       </c>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K10" s="14" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>49</v>
+        <v>76</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -1468,20 +1461,20 @@
         <v>3</v>
       </c>
       <c r="E11" t="s">
-        <v>50</v>
+        <v>77</v>
       </c>
       <c r="G11" t="s">
-        <v>19</v>
+        <v>78</v>
       </c>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>62</v>
+        <v>17</v>
       </c>
       <c r="B12" t="s">
-        <v>65</v>
+        <v>48</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -1491,20 +1484,20 @@
         <v>3</v>
       </c>
       <c r="E12" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="G12" t="s">
-        <v>63</v>
+        <v>19</v>
       </c>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>52</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>53</v>
+        <v>18</v>
+      </c>
+      <c r="B13" t="s">
+        <v>49</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -1514,23 +1507,20 @@
         <v>3</v>
       </c>
       <c r="E13" t="s">
-        <v>54</v>
-      </c>
-      <c r="F13" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="G13" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>57</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>108</v>
+        <v>62</v>
+      </c>
+      <c r="B14" t="s">
+        <v>65</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -1540,85 +1530,85 @@
         <v>3</v>
       </c>
       <c r="E14" t="s">
-        <v>14</v>
-      </c>
-      <c r="F14" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="G14" t="s">
-        <v>13</v>
+        <v>63</v>
       </c>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>79</v>
-      </c>
-      <c r="B15" t="s">
-        <v>109</v>
+        <v>52</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>53</v>
       </c>
       <c r="C15">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="D15">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="E15" t="s">
-        <v>20</v>
+        <v>54</v>
       </c>
       <c r="F15" t="s">
-        <v>21</v>
+        <v>55</v>
       </c>
       <c r="G15" t="s">
-        <v>22</v>
+        <v>56</v>
       </c>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>80</v>
-      </c>
-      <c r="B16" t="s">
-        <v>110</v>
+        <v>57</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>108</v>
       </c>
       <c r="C16">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D16">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="E16" t="s">
         <v>14</v>
       </c>
       <c r="F16" t="s">
-        <v>31</v>
+        <v>58</v>
       </c>
       <c r="G16" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>61</v>
+        <v>79</v>
       </c>
       <c r="B17" t="s">
-        <v>23</v>
+        <v>109</v>
       </c>
       <c r="C17">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="D17">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="E17" t="s">
-        <v>24</v>
+        <v>20</v>
+      </c>
+      <c r="F17" t="s">
+        <v>21</v>
       </c>
       <c r="G17" t="s">
         <v>22</v>
@@ -1626,25 +1616,25 @@
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="B18" t="s">
-        <v>28</v>
+        <v>110</v>
       </c>
       <c r="C18">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D18">
         <f t="shared" si="0"/>
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="E18" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="F18" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="G18" t="s">
         <v>22</v>
@@ -1652,12 +1642,12 @@
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>66</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>67</v>
+        <v>61</v>
+      </c>
+      <c r="B19" t="s">
+        <v>23</v>
       </c>
       <c r="C19">
         <v>2</v>
@@ -1667,10 +1657,7 @@
         <v>6</v>
       </c>
       <c r="E19" t="s">
-        <v>25</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>68</v>
+        <v>24</v>
       </c>
       <c r="G19" t="s">
         <v>22</v>
@@ -1678,25 +1665,25 @@
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>92</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>29</v>
+        <v>91</v>
+      </c>
+      <c r="B20" t="s">
+        <v>28</v>
       </c>
       <c r="C20">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D20">
-        <f>C20*D$1</f>
-        <v>9</v>
+        <f t="shared" si="0"/>
+        <v>21</v>
       </c>
       <c r="E20" t="s">
         <v>25</v>
       </c>
-      <c r="F20" s="3" t="s">
-        <v>27</v>
+      <c r="F20" t="s">
+        <v>26</v>
       </c>
       <c r="G20" t="s">
         <v>22</v>
@@ -1704,25 +1691,25 @@
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>81</v>
+        <v>66</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D21">
-        <f>C21*D$1</f>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>6</v>
       </c>
       <c r="E21" t="s">
         <v>25</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G21" t="s">
         <v>22</v>
@@ -1730,225 +1717,1051 @@
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>72</v>
+        <v>29</v>
       </c>
       <c r="C22">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D22">
-        <f>C22*D$1</f>
-        <v>3</v>
+        <f>C22*D$3</f>
+        <v>9</v>
       </c>
       <c r="E22" t="s">
         <v>25</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>74</v>
+        <v>27</v>
       </c>
       <c r="G22" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>30</v>
+        <v>81</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C23">
         <v>1</v>
       </c>
       <c r="D23">
-        <f>C23*D$1</f>
+        <f>C23*D$3</f>
         <v>3</v>
       </c>
       <c r="E23" t="s">
         <v>25</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="G23" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>89</v>
+        <v>72</v>
       </c>
       <c r="C24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D24">
-        <f>C24*D$1</f>
-        <v>6</v>
+        <f>C24*D$3</f>
+        <v>3</v>
       </c>
       <c r="E24" t="s">
-        <v>86</v>
+        <v>25</v>
       </c>
       <c r="F24" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="G24" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>30</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25">
+        <f>C25*D$3</f>
+        <v>3</v>
+      </c>
+      <c r="E25" t="s">
+        <v>25</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="G25" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>112</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C26">
+        <v>3</v>
+      </c>
+      <c r="D26">
+        <f>C26*D$3</f>
+        <v>9</v>
+      </c>
+      <c r="E26" t="s">
+        <v>25</v>
+      </c>
+      <c r="F26" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="G24" t="s">
-        <v>87</v>
-      </c>
-      <c r="H24" t="s">
-        <v>88</v>
-      </c>
-      <c r="I24" s="1"/>
-      <c r="J24" s="1"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="I25" s="1"/>
-      <c r="J25" s="1"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A26" s="5" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G26" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>96</v>
-      </c>
-      <c r="B27" t="s">
-        <v>97</v>
-      </c>
+        <v>113</v>
+      </c>
+      <c r="B27" s="2"/>
       <c r="C27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D27">
-        <f>C27*D$1</f>
-        <v>3</v>
+        <f>C27*D$3</f>
+        <v>0</v>
       </c>
       <c r="E27" t="s">
-        <v>98</v>
-      </c>
-      <c r="F27" t="s">
-        <v>99</v>
+        <v>114</v>
+      </c>
+      <c r="F27" s="3"/>
+      <c r="G27" t="s">
+        <v>13</v>
+      </c>
+      <c r="H27" t="s">
+        <v>115</v>
       </c>
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A28" s="17" t="s">
-        <v>101</v>
-      </c>
-      <c r="B28" s="16" t="s">
-        <v>102</v>
-      </c>
-      <c r="C28">
-        <v>1</v>
-      </c>
-      <c r="D28">
-        <f>C28*D$1</f>
-        <v>3</v>
-      </c>
-      <c r="E28" t="s">
-        <v>103</v>
-      </c>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A29" s="17"/>
-      <c r="B29" s="3" t="s">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>96</v>
+      </c>
+      <c r="B30" t="s">
+        <v>97</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="D30">
+        <f>C30*D$3</f>
+        <v>3</v>
+      </c>
+      <c r="E30" t="s">
+        <v>98</v>
+      </c>
+      <c r="F30" t="s">
+        <v>99</v>
+      </c>
+      <c r="I30" s="1"/>
+      <c r="J30" s="1"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="B31" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
+      <c r="D31">
+        <f>C31*D$3</f>
+        <v>3</v>
+      </c>
+      <c r="E31" t="s">
+        <v>103</v>
+      </c>
+      <c r="I31" s="1"/>
+      <c r="J31" s="1"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" s="17"/>
+      <c r="B32" s="3" t="s">
         <v>104</v>
       </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="D32">
+        <f>C32*D$3</f>
+        <v>3</v>
+      </c>
+      <c r="E32" t="s">
+        <v>106</v>
+      </c>
+      <c r="I32" s="1"/>
+      <c r="J32" s="1"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" s="17"/>
+      <c r="B33" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C33">
+        <v>2</v>
+      </c>
+      <c r="D33">
+        <f>C33*D$3</f>
+        <v>6</v>
+      </c>
+      <c r="E33" t="s">
+        <v>107</v>
+      </c>
+      <c r="F33" s="3"/>
+      <c r="I33" s="1"/>
+      <c r="J33" s="1"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B34" s="2"/>
+      <c r="I34" s="1"/>
+      <c r="J34" s="1"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F35" s="3"/>
+      <c r="I35" s="1"/>
+      <c r="J35" s="1"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F36" s="3"/>
+      <c r="I36" s="1"/>
+      <c r="J36" s="1"/>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F37" s="3"/>
+      <c r="I37" s="1"/>
+      <c r="J37" s="1"/>
+    </row>
+    <row r="38" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F38" s="8"/>
+      <c r="H38" s="6"/>
+      <c r="I38" s="9"/>
+      <c r="J38" s="10"/>
+    </row>
+    <row r="39" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="11"/>
+      <c r="F39" s="8"/>
+      <c r="H39" s="6"/>
+      <c r="I39" s="9"/>
+      <c r="J39" s="10"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F40" s="3"/>
+      <c r="H40" s="2"/>
+      <c r="I40" s="4"/>
+      <c r="J40" s="1"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I42" s="1"/>
+      <c r="J42" s="1"/>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B43" s="1"/>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B44" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A31:A33"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K43"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="17.85546875" customWidth="1"/>
+    <col min="5" max="5" width="23.42578125" customWidth="1"/>
+    <col min="8" max="8" width="59.85546875" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="18" t="s">
+        <v>116</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <f>C6*D$3</f>
+        <v>3</v>
+      </c>
+      <c r="E6" t="s">
+        <v>33</v>
+      </c>
+      <c r="G6" t="s">
+        <v>34</v>
+      </c>
+      <c r="H6" t="s">
+        <v>36</v>
+      </c>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <f t="shared" ref="D7:D21" si="0">C7*D$3</f>
+        <v>3</v>
+      </c>
+      <c r="E7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G7" t="s">
+        <v>34</v>
+      </c>
+      <c r="H7" t="s">
+        <v>38</v>
+      </c>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E8" t="s">
+        <v>40</v>
+      </c>
+      <c r="G8" t="s">
+        <v>41</v>
+      </c>
+      <c r="H8" t="s">
+        <v>42</v>
+      </c>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
+        <v>90</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E9" t="s">
+        <v>47</v>
+      </c>
+      <c r="G9" t="s">
+        <v>94</v>
+      </c>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E10" t="s">
+        <v>44</v>
+      </c>
+      <c r="G10" t="s">
+        <v>45</v>
+      </c>
+      <c r="H10" t="s">
+        <v>46</v>
+      </c>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="14" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" t="s">
+        <v>76</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E11" t="s">
+        <v>77</v>
+      </c>
+      <c r="G11" t="s">
+        <v>78</v>
+      </c>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E12" t="s">
+        <v>51</v>
+      </c>
+      <c r="G12" t="s">
+        <v>19</v>
+      </c>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" t="s">
+        <v>49</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E13" t="s">
+        <v>50</v>
+      </c>
+      <c r="G13" t="s">
+        <v>19</v>
+      </c>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>62</v>
+      </c>
+      <c r="B14" t="s">
+        <v>65</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E14" t="s">
+        <v>64</v>
+      </c>
+      <c r="G14" t="s">
+        <v>63</v>
+      </c>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>52</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E15" t="s">
+        <v>54</v>
+      </c>
+      <c r="F15" t="s">
+        <v>55</v>
+      </c>
+      <c r="G15" t="s">
+        <v>56</v>
+      </c>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>57</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E16" t="s">
+        <v>14</v>
+      </c>
+      <c r="F16" t="s">
+        <v>58</v>
+      </c>
+      <c r="G16" t="s">
+        <v>13</v>
+      </c>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>79</v>
+      </c>
+      <c r="B17" t="s">
+        <v>109</v>
+      </c>
+      <c r="C17">
+        <v>10</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="E17" t="s">
+        <v>20</v>
+      </c>
+      <c r="F17" t="s">
+        <v>21</v>
+      </c>
+      <c r="G17" t="s">
+        <v>22</v>
+      </c>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>80</v>
+      </c>
+      <c r="B18" t="s">
+        <v>110</v>
+      </c>
+      <c r="C18">
+        <v>4</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="E18" t="s">
+        <v>14</v>
+      </c>
+      <c r="F18" t="s">
+        <v>31</v>
+      </c>
+      <c r="G18" t="s">
+        <v>22</v>
+      </c>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>61</v>
+      </c>
+      <c r="B19" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19">
+        <v>2</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="E19" t="s">
+        <v>24</v>
+      </c>
+      <c r="G19" t="s">
+        <v>22</v>
+      </c>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>91</v>
+      </c>
+      <c r="B20" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20">
+        <v>7</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="E20" t="s">
+        <v>25</v>
+      </c>
+      <c r="F20" t="s">
+        <v>26</v>
+      </c>
+      <c r="G20" t="s">
+        <v>22</v>
+      </c>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>66</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C21">
+        <v>2</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="E21" t="s">
+        <v>25</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="G21" t="s">
+        <v>22</v>
+      </c>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>92</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22">
+        <v>3</v>
+      </c>
+      <c r="D22">
+        <f>C22*D$3</f>
+        <v>9</v>
+      </c>
+      <c r="E22" t="s">
+        <v>25</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G22" t="s">
+        <v>22</v>
+      </c>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>81</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <f>C23*D$3</f>
+        <v>3</v>
+      </c>
+      <c r="E23" t="s">
+        <v>25</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="G23" t="s">
+        <v>22</v>
+      </c>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>93</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24">
+        <f>C24*D$3</f>
+        <v>3</v>
+      </c>
+      <c r="E24" t="s">
+        <v>25</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="G24" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>30</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25">
+        <f>C25*D$3</f>
+        <v>3</v>
+      </c>
+      <c r="E25" t="s">
+        <v>25</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="G25" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>85</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C26">
+        <v>2</v>
+      </c>
+      <c r="D26">
+        <f>C26*D$3</f>
+        <v>6</v>
+      </c>
+      <c r="E26" t="s">
+        <v>86</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G26" t="s">
+        <v>87</v>
+      </c>
+      <c r="H26" t="s">
+        <v>88</v>
+      </c>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>96</v>
+      </c>
+      <c r="B29" t="s">
+        <v>97</v>
+      </c>
       <c r="C29">
         <v>1</v>
       </c>
       <c r="D29">
-        <f>C29*D$1</f>
+        <f>C29*D$3</f>
         <v>3</v>
       </c>
       <c r="E29" t="s">
-        <v>106</v>
+        <v>98</v>
+      </c>
+      <c r="F29" t="s">
+        <v>99</v>
       </c>
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A30" s="17"/>
-      <c r="B30" s="2" t="s">
-        <v>105</v>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="B30" s="15" t="s">
+        <v>102</v>
       </c>
       <c r="C30">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D30">
-        <f>C30*D$1</f>
-        <v>6</v>
+        <f>C30*D$3</f>
+        <v>3</v>
       </c>
       <c r="E30" t="s">
-        <v>107</v>
-      </c>
-      <c r="F30" s="3"/>
+        <v>103</v>
+      </c>
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B31" s="2"/>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" s="17"/>
+      <c r="B31" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
+      <c r="D31">
+        <f>C31*D$3</f>
+        <v>3</v>
+      </c>
+      <c r="E31" t="s">
+        <v>106</v>
+      </c>
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" s="17"/>
+      <c r="B32" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C32">
+        <v>2</v>
+      </c>
+      <c r="D32">
+        <f>C32*D$3</f>
+        <v>6</v>
+      </c>
+      <c r="E32" t="s">
+        <v>107</v>
+      </c>
       <c r="F32" s="3"/>
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
     </row>
-    <row r="33" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="F33" s="3"/>
+    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B33" s="2"/>
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
     </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
       <c r="F34" s="3"/>
       <c r="I34" s="1"/>
       <c r="J34" s="1"/>
     </row>
-    <row r="35" spans="2:10" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="F35" s="8"/>
-      <c r="H35" s="6"/>
-      <c r="I35" s="9"/>
-      <c r="J35" s="10"/>
-    </row>
-    <row r="36" spans="2:10" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="11"/>
-      <c r="F36" s="8"/>
-      <c r="H36" s="6"/>
-      <c r="I36" s="9"/>
-      <c r="J36" s="10"/>
-    </row>
-    <row r="37" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="F37" s="3"/>
-      <c r="H37" s="2"/>
-      <c r="I37" s="4"/>
-      <c r="J37" s="1"/>
-    </row>
-    <row r="39" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="I39" s="1"/>
+    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="F35" s="3"/>
+      <c r="I35" s="1"/>
+      <c r="J35" s="1"/>
+    </row>
+    <row r="36" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="F36" s="3"/>
+      <c r="I36" s="1"/>
+      <c r="J36" s="1"/>
+    </row>
+    <row r="37" spans="2:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F37" s="8"/>
+      <c r="H37" s="6"/>
+      <c r="I37" s="9"/>
+      <c r="J37" s="10"/>
+    </row>
+    <row r="38" spans="2:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="11"/>
+      <c r="F38" s="8"/>
+      <c r="H38" s="6"/>
+      <c r="I38" s="9"/>
+      <c r="J38" s="10"/>
+    </row>
+    <row r="39" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="F39" s="3"/>
+      <c r="H39" s="2"/>
+      <c r="I39" s="4"/>
       <c r="J39" s="1"/>
     </row>
-    <row r="40" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B40" s="1"/>
-    </row>
-    <row r="41" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B41" s="1"/>
+    <row r="41" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I41" s="1"/>
+      <c r="J41" s="1"/>
+    </row>
+    <row r="42" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B42" s="1"/>
+    </row>
+    <row r="43" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B43" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A28:A30"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A30:A32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update PCB design: - selectable sync level for the buffered output - video buffer for sync instead of transistor
</commit_message>
<xml_diff>
--- a/MultiRegion_with_DeJitter_QID/BOM.xlsx
+++ b/MultiRegion_with_DeJitter_QID/BOM.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="d:\Users\Peter\Documents\Workspaces\Git\SNES-AddOn-PCBs\MultiRegion_with_DeJitter_QID\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Peter\Documents\Workspaces\Git\Eigenes\SNES-AddOn-PCBs\MultiRegion_with_DeJitter_QID\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D342493C-A023-4098-A726-C06D93E42466}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7BD5819-92A9-4FFB-A869-D3A774597145}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8850" yWindow="3120" windowWidth="23955" windowHeight="16320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="SMR20190813" sheetId="4" r:id="rId1"/>
-    <sheet name="SMR20190603" sheetId="3" r:id="rId2"/>
+    <sheet name="SMR20200323" sheetId="5" r:id="rId1"/>
+    <sheet name="SMR20190813" sheetId="4" r:id="rId2"/>
+    <sheet name="SMR20190603" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029" refMode="R1C1"/>
+  <calcPr calcId="181029" refMode="R1C1" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="330"/>
@@ -24,6 +25,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="150">
   <si>
     <t>Designator</t>
   </si>
@@ -394,6 +396,96 @@
   </si>
   <si>
     <t>(and earlier)</t>
+  </si>
+  <si>
+    <t>U9</t>
+  </si>
+  <si>
+    <t>TSH122ICT</t>
+  </si>
+  <si>
+    <t>Video Driver, 6dB, 1 Ch.</t>
+  </si>
+  <si>
+    <t>SC-70-6</t>
+  </si>
+  <si>
+    <t>C91</t>
+  </si>
+  <si>
+    <t>C92</t>
+  </si>
+  <si>
+    <t>(10uF cap 0603)</t>
+  </si>
+  <si>
+    <t>(10nF cap 0603)</t>
+  </si>
+  <si>
+    <t>10uF /  25V</t>
+  </si>
+  <si>
+    <t>0.01uF / 50V</t>
+  </si>
+  <si>
+    <t>(22uF cap 0603)</t>
+  </si>
+  <si>
+    <t>C93</t>
+  </si>
+  <si>
+    <t>(33uF cap 0805)</t>
+  </si>
+  <si>
+    <t>33uF / 5V</t>
+  </si>
+  <si>
+    <t>R11,R21,R32,R38,R39,R52</t>
+  </si>
+  <si>
+    <t>R31,R37</t>
+  </si>
+  <si>
+    <t>C1,C94</t>
+  </si>
+  <si>
+    <t>R91</t>
+  </si>
+  <si>
+    <t>R92</t>
+  </si>
+  <si>
+    <t>R93</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RC0603FR-0775RL </t>
+  </si>
+  <si>
+    <t>RC0603FR-074K7L</t>
+  </si>
+  <si>
+    <t>4.7k</t>
+  </si>
+  <si>
+    <t>75</t>
+  </si>
+  <si>
+    <t>R94</t>
+  </si>
+  <si>
+    <t>SMR20200323</t>
+  </si>
+  <si>
+    <t>6.19k</t>
+  </si>
+  <si>
+    <t>523</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RC0603FR-07523RL </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RC0603FR-076K19L </t>
   </si>
 </sst>
 </file>
@@ -1245,28 +1337,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K44"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56AAEB05-E62E-4D9F-8ABF-51FB4F1B6F14}">
+  <dimension ref="A1:K49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.88671875" customWidth="1"/>
-    <col min="5" max="5" width="23.44140625" customWidth="1"/>
-    <col min="8" max="8" width="59.88671875" customWidth="1"/>
-    <col min="9" max="9" width="11.33203125" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" customWidth="1"/>
+    <col min="5" max="5" width="23.42578125" customWidth="1"/>
+    <col min="8" max="8" width="59.85546875" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
         <v>116</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
         <v>59</v>
       </c>
@@ -1276,7 +1368,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>0</v>
       </c>
@@ -1311,7 +1403,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -1340,7 +1432,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -1351,7 +1443,7 @@
         <v>1</v>
       </c>
       <c r="D7">
-        <f t="shared" ref="D7:D21" si="0">C7*D$3</f>
+        <f t="shared" ref="D7:D32" si="0">C7*D$3</f>
         <v>3</v>
       </c>
       <c r="E7" t="s">
@@ -1369,7 +1461,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -1398,7 +1490,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -1421,7 +1513,7 @@
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -1450,7 +1542,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -1473,7 +1565,7 @@
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -1496,7 +1588,7 @@
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -1519,7 +1611,913 @@
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>120</v>
+      </c>
+      <c r="B14" t="s">
+        <v>121</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E14" t="s">
+        <v>122</v>
+      </c>
+      <c r="G14" t="s">
+        <v>123</v>
+      </c>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>52</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E15" t="s">
+        <v>54</v>
+      </c>
+      <c r="F15" t="s">
+        <v>55</v>
+      </c>
+      <c r="G15" t="s">
+        <v>56</v>
+      </c>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>136</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C16">
+        <v>2</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="E16" t="s">
+        <v>14</v>
+      </c>
+      <c r="F16" t="s">
+        <v>58</v>
+      </c>
+      <c r="G16" t="s">
+        <v>22</v>
+      </c>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>79</v>
+      </c>
+      <c r="B17" t="s">
+        <v>109</v>
+      </c>
+      <c r="C17">
+        <v>10</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="E17" t="s">
+        <v>20</v>
+      </c>
+      <c r="F17" t="s">
+        <v>21</v>
+      </c>
+      <c r="G17" t="s">
+        <v>22</v>
+      </c>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>80</v>
+      </c>
+      <c r="B18" t="s">
+        <v>110</v>
+      </c>
+      <c r="C18">
+        <v>4</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="E18" t="s">
+        <v>14</v>
+      </c>
+      <c r="F18" t="s">
+        <v>31</v>
+      </c>
+      <c r="G18" t="s">
+        <v>22</v>
+      </c>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>124</v>
+      </c>
+      <c r="B19" t="s">
+        <v>126</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E19" t="s">
+        <v>14</v>
+      </c>
+      <c r="F19" t="s">
+        <v>128</v>
+      </c>
+      <c r="G19" t="s">
+        <v>22</v>
+      </c>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>125</v>
+      </c>
+      <c r="B20" t="s">
+        <v>127</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E20" t="s">
+        <v>20</v>
+      </c>
+      <c r="F20" t="s">
+        <v>129</v>
+      </c>
+      <c r="G20" t="s">
+        <v>22</v>
+      </c>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>131</v>
+      </c>
+      <c r="B21" t="s">
+        <v>132</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E21" t="s">
+        <v>14</v>
+      </c>
+      <c r="F21" t="s">
+        <v>133</v>
+      </c>
+      <c r="G21" t="s">
+        <v>13</v>
+      </c>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>61</v>
+      </c>
+      <c r="B22" t="s">
+        <v>23</v>
+      </c>
+      <c r="C22">
+        <v>2</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="E22" t="s">
+        <v>24</v>
+      </c>
+      <c r="G22" t="s">
+        <v>22</v>
+      </c>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>134</v>
+      </c>
+      <c r="B23" t="s">
+        <v>28</v>
+      </c>
+      <c r="C23">
+        <v>6</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="E23" t="s">
+        <v>25</v>
+      </c>
+      <c r="F23" t="s">
+        <v>26</v>
+      </c>
+      <c r="G23" t="s">
+        <v>22</v>
+      </c>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>66</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C24">
+        <v>2</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="E24" t="s">
+        <v>25</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="G24" t="s">
+        <v>22</v>
+      </c>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>135</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C25">
+        <v>2</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="E25" t="s">
+        <v>25</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G25" t="s">
+        <v>22</v>
+      </c>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>30</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E26" t="s">
+        <v>25</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="G26" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>112</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C27">
+        <v>3</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="E27" t="s">
+        <v>25</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G27" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>113</v>
+      </c>
+      <c r="B28" s="2"/>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E28" t="s">
+        <v>114</v>
+      </c>
+      <c r="F28" s="3"/>
+      <c r="G28" t="s">
+        <v>13</v>
+      </c>
+      <c r="H28" t="s">
+        <v>115</v>
+      </c>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>137</v>
+      </c>
+      <c r="B29" t="s">
+        <v>141</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E29" t="s">
+        <v>25</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="G29" t="s">
+        <v>22</v>
+      </c>
+      <c r="I29" s="1"/>
+      <c r="J29" s="1"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>138</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E30" t="s">
+        <v>25</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="G30" t="s">
+        <v>22</v>
+      </c>
+      <c r="I30" s="1"/>
+      <c r="J30" s="1"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>139</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
+      <c r="D31">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E31" t="s">
+        <v>25</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="G31" t="s">
+        <v>22</v>
+      </c>
+      <c r="I31" s="1"/>
+      <c r="J31" s="1"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>144</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="D32">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E32" t="s">
+        <v>25</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="G32" t="s">
+        <v>22</v>
+      </c>
+      <c r="I32" s="1"/>
+      <c r="J32" s="1"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I33" s="1"/>
+      <c r="J33" s="1"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>96</v>
+      </c>
+      <c r="B35" t="s">
+        <v>97</v>
+      </c>
+      <c r="C35">
+        <v>1</v>
+      </c>
+      <c r="D35">
+        <f>C35*D$3</f>
+        <v>3</v>
+      </c>
+      <c r="E35" t="s">
+        <v>98</v>
+      </c>
+      <c r="F35" t="s">
+        <v>99</v>
+      </c>
+      <c r="I35" s="1"/>
+      <c r="J35" s="1"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="B36" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="C36">
+        <v>1</v>
+      </c>
+      <c r="D36">
+        <f>C36*D$3</f>
+        <v>3</v>
+      </c>
+      <c r="E36" t="s">
+        <v>103</v>
+      </c>
+      <c r="I36" s="1"/>
+      <c r="J36" s="1"/>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" s="18"/>
+      <c r="B37" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C37">
+        <v>1</v>
+      </c>
+      <c r="D37">
+        <f>C37*D$3</f>
+        <v>3</v>
+      </c>
+      <c r="E37" t="s">
+        <v>106</v>
+      </c>
+      <c r="I37" s="1"/>
+      <c r="J37" s="1"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38" s="18"/>
+      <c r="B38" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C38">
+        <v>2</v>
+      </c>
+      <c r="D38">
+        <f>C38*D$3</f>
+        <v>6</v>
+      </c>
+      <c r="E38" t="s">
+        <v>107</v>
+      </c>
+      <c r="F38" s="3"/>
+      <c r="I38" s="1"/>
+      <c r="J38" s="1"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B39" s="2"/>
+      <c r="I39" s="1"/>
+      <c r="J39" s="1"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F40" s="3"/>
+      <c r="I40" s="1"/>
+      <c r="J40" s="1"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F41" s="3"/>
+      <c r="I41" s="1"/>
+      <c r="J41" s="1"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F42" s="3"/>
+      <c r="I42" s="1"/>
+      <c r="J42" s="1"/>
+    </row>
+    <row r="43" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F43" s="8"/>
+      <c r="H43" s="6"/>
+      <c r="I43" s="9"/>
+      <c r="J43" s="10"/>
+    </row>
+    <row r="44" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="11"/>
+      <c r="F44" s="8"/>
+      <c r="H44" s="6"/>
+      <c r="I44" s="9"/>
+      <c r="J44" s="10"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F45" s="3"/>
+      <c r="H45" s="2"/>
+      <c r="I45" s="4"/>
+      <c r="J45" s="1"/>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I47" s="1"/>
+      <c r="J47" s="1"/>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B48" s="1"/>
+    </row>
+    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B49" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A36:A38"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K44"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="17.85546875" customWidth="1"/>
+    <col min="5" max="5" width="23.42578125" customWidth="1"/>
+    <col min="8" max="8" width="59.85546875" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <f>C6*D$3</f>
+        <v>3</v>
+      </c>
+      <c r="E6" t="s">
+        <v>33</v>
+      </c>
+      <c r="G6" t="s">
+        <v>34</v>
+      </c>
+      <c r="H6" t="s">
+        <v>36</v>
+      </c>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <f t="shared" ref="D7:D21" si="0">C7*D$3</f>
+        <v>3</v>
+      </c>
+      <c r="E7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G7" t="s">
+        <v>34</v>
+      </c>
+      <c r="H7" t="s">
+        <v>38</v>
+      </c>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E8" t="s">
+        <v>40</v>
+      </c>
+      <c r="G8" t="s">
+        <v>41</v>
+      </c>
+      <c r="H8" t="s">
+        <v>42</v>
+      </c>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
+        <v>90</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E9" t="s">
+        <v>47</v>
+      </c>
+      <c r="G9" t="s">
+        <v>94</v>
+      </c>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E10" t="s">
+        <v>44</v>
+      </c>
+      <c r="G10" t="s">
+        <v>45</v>
+      </c>
+      <c r="H10" t="s">
+        <v>46</v>
+      </c>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="14" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" t="s">
+        <v>76</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E11" t="s">
+        <v>77</v>
+      </c>
+      <c r="G11" t="s">
+        <v>78</v>
+      </c>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E12" t="s">
+        <v>51</v>
+      </c>
+      <c r="G12" t="s">
+        <v>19</v>
+      </c>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" t="s">
+        <v>49</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E13" t="s">
+        <v>50</v>
+      </c>
+      <c r="G13" t="s">
+        <v>19</v>
+      </c>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>62</v>
       </c>
@@ -1542,7 +2540,7 @@
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>52</v>
       </c>
@@ -1568,7 +2566,7 @@
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>57</v>
       </c>
@@ -1594,7 +2592,7 @@
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>79</v>
       </c>
@@ -1620,7 +2618,7 @@
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>80</v>
       </c>
@@ -1646,7 +2644,7 @@
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>61</v>
       </c>
@@ -1669,7 +2667,7 @@
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>91</v>
       </c>
@@ -1695,7 +2693,7 @@
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>66</v>
       </c>
@@ -1721,7 +2719,7 @@
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>92</v>
       </c>
@@ -1747,7 +2745,7 @@
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>81</v>
       </c>
@@ -1773,7 +2771,7 @@
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>93</v>
       </c>
@@ -1797,7 +2795,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>30</v>
       </c>
@@ -1821,7 +2819,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>112</v>
       </c>
@@ -1845,7 +2843,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>113</v>
       </c>
@@ -1870,16 +2868,16 @@
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>96</v>
       </c>
@@ -1902,7 +2900,7 @@
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="18" t="s">
         <v>101</v>
       </c>
@@ -1922,7 +2920,7 @@
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="18"/>
       <c r="B32" s="3" t="s">
         <v>104</v>
@@ -1940,7 +2938,7 @@
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="18"/>
       <c r="B33" s="2" t="s">
         <v>105</v>
@@ -1959,53 +2957,53 @@
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B34" s="2"/>
       <c r="I34" s="1"/>
       <c r="J34" s="1"/>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F35" s="3"/>
       <c r="I35" s="1"/>
       <c r="J35" s="1"/>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F36" s="3"/>
       <c r="I36" s="1"/>
       <c r="J36" s="1"/>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F37" s="3"/>
       <c r="I37" s="1"/>
       <c r="J37" s="1"/>
     </row>
-    <row r="38" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F38" s="8"/>
       <c r="H38" s="6"/>
       <c r="I38" s="9"/>
       <c r="J38" s="10"/>
     </row>
-    <row r="39" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B39" s="11"/>
       <c r="F39" s="8"/>
       <c r="H39" s="6"/>
       <c r="I39" s="9"/>
       <c r="J39" s="10"/>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F40" s="3"/>
       <c r="H40" s="2"/>
       <c r="I40" s="4"/>
       <c r="J40" s="1"/>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I42" s="1"/>
       <c r="J42" s="1"/>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B43" s="1"/>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B44" s="1"/>
     </row>
   </sheetData>
@@ -2018,21 +3016,21 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K43"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.88671875" customWidth="1"/>
-    <col min="5" max="5" width="23.44140625" customWidth="1"/>
-    <col min="8" max="8" width="59.88671875" customWidth="1"/>
-    <col min="9" max="9" width="11.33203125" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" customWidth="1"/>
+    <col min="5" max="5" width="23.42578125" customWidth="1"/>
+    <col min="8" max="8" width="59.85546875" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
         <v>116</v>
       </c>
@@ -2043,7 +3041,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
         <v>59</v>
       </c>
@@ -2053,7 +3051,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>0</v>
       </c>
@@ -2088,7 +3086,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -2117,7 +3115,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -2146,7 +3144,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -2175,7 +3173,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -2198,7 +3196,7 @@
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -2227,7 +3225,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -2250,7 +3248,7 @@
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -2273,7 +3271,7 @@
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -2296,7 +3294,7 @@
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>62</v>
       </c>
@@ -2319,7 +3317,7 @@
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>52</v>
       </c>
@@ -2345,7 +3343,7 @@
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>57</v>
       </c>
@@ -2371,7 +3369,7 @@
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>79</v>
       </c>
@@ -2397,7 +3395,7 @@
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>80</v>
       </c>
@@ -2423,7 +3421,7 @@
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>61</v>
       </c>
@@ -2446,7 +3444,7 @@
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>91</v>
       </c>
@@ -2472,7 +3470,7 @@
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>66</v>
       </c>
@@ -2498,7 +3496,7 @@
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>92</v>
       </c>
@@ -2524,7 +3522,7 @@
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>81</v>
       </c>
@@ -2550,7 +3548,7 @@
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>93</v>
       </c>
@@ -2574,7 +3572,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>30</v>
       </c>
@@ -2598,7 +3596,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>85</v>
       </c>
@@ -2627,16 +3625,16 @@
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>96</v>
       </c>
@@ -2659,7 +3657,7 @@
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="18" t="s">
         <v>101</v>
       </c>
@@ -2679,7 +3677,7 @@
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="18"/>
       <c r="B31" s="3" t="s">
         <v>104</v>
@@ -2697,7 +3695,7 @@
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="18"/>
       <c r="B32" s="2" t="s">
         <v>105</v>
@@ -2716,53 +3714,53 @@
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
     </row>
-    <row r="33" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B33" s="2"/>
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
     </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
       <c r="F34" s="3"/>
       <c r="I34" s="1"/>
       <c r="J34" s="1"/>
     </row>
-    <row r="35" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
       <c r="F35" s="3"/>
       <c r="I35" s="1"/>
       <c r="J35" s="1"/>
     </row>
-    <row r="36" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:10" x14ac:dyDescent="0.25">
       <c r="F36" s="3"/>
       <c r="I36" s="1"/>
       <c r="J36" s="1"/>
     </row>
-    <row r="37" spans="2:10" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F37" s="8"/>
       <c r="H37" s="6"/>
       <c r="I37" s="9"/>
       <c r="J37" s="10"/>
     </row>
-    <row r="38" spans="2:10" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B38" s="11"/>
       <c r="F38" s="8"/>
       <c r="H38" s="6"/>
       <c r="I38" s="9"/>
       <c r="J38" s="10"/>
     </row>
-    <row r="39" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:10" x14ac:dyDescent="0.25">
       <c r="F39" s="3"/>
       <c r="H39" s="2"/>
       <c r="I39" s="4"/>
       <c r="J39" s="1"/>
     </row>
-    <row r="41" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:10" x14ac:dyDescent="0.25">
       <c r="I41" s="1"/>
       <c r="J41" s="1"/>
     </row>
-    <row r="42" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B42" s="1"/>
     </row>
-    <row r="43" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B43" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update PCB design: - selectable sync level for the buffered output - video buffer for sync instead of transistor - color carrier fix applied - some GND between sub-carrier and master clock output
</commit_message>
<xml_diff>
--- a/MultiRegion_with_DeJitter_QID/BOM.xlsx
+++ b/MultiRegion_with_DeJitter_QID/BOM.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21901"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="d:\Users\Peter\Documents\Workspaces\Git\SNES-AddOn-PCBs\MultiRegion_with_DeJitter_QID\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UserData\Bartmann\Workspaces\Git\Eigenes\SNES-AddOn-PCBs\MultiRegion_with_DeJitter_QID\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D342493C-A023-4098-A726-C06D93E42466}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8850" yWindow="3120" windowWidth="23955" windowHeight="16320"/>
   </bookViews>
   <sheets>
-    <sheet name="SMR20190813" sheetId="4" r:id="rId1"/>
-    <sheet name="SMR20190603" sheetId="3" r:id="rId2"/>
+    <sheet name="SMR20200325" sheetId="5" r:id="rId1"/>
+    <sheet name="SMR20190813" sheetId="4" r:id="rId2"/>
+    <sheet name="SMR20190603" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029" refMode="R1C1"/>
+  <calcPr calcId="162913" refMode="R1C1" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="330"/>
@@ -24,6 +24,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="150">
   <si>
     <t>Designator</t>
   </si>
@@ -394,12 +395,102 @@
   </si>
   <si>
     <t>(and earlier)</t>
+  </si>
+  <si>
+    <t>U9</t>
+  </si>
+  <si>
+    <t>TSH122ICT</t>
+  </si>
+  <si>
+    <t>Video Driver, 6dB, 1 Ch.</t>
+  </si>
+  <si>
+    <t>SC-70-6</t>
+  </si>
+  <si>
+    <t>C91</t>
+  </si>
+  <si>
+    <t>C92</t>
+  </si>
+  <si>
+    <t>(10uF cap 0603)</t>
+  </si>
+  <si>
+    <t>(10nF cap 0603)</t>
+  </si>
+  <si>
+    <t>10uF /  25V</t>
+  </si>
+  <si>
+    <t>0.01uF / 50V</t>
+  </si>
+  <si>
+    <t>(22uF cap 0603)</t>
+  </si>
+  <si>
+    <t>C93</t>
+  </si>
+  <si>
+    <t>(33uF cap 0805)</t>
+  </si>
+  <si>
+    <t>33uF / 5V</t>
+  </si>
+  <si>
+    <t>R31,R37</t>
+  </si>
+  <si>
+    <t>C1,C94</t>
+  </si>
+  <si>
+    <t>R91</t>
+  </si>
+  <si>
+    <t>R92</t>
+  </si>
+  <si>
+    <t>R93</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RC0603FR-0775RL </t>
+  </si>
+  <si>
+    <t>RC0603FR-074K7L</t>
+  </si>
+  <si>
+    <t>4.7k</t>
+  </si>
+  <si>
+    <t>75</t>
+  </si>
+  <si>
+    <t>R94</t>
+  </si>
+  <si>
+    <t>6.19k</t>
+  </si>
+  <si>
+    <t>523</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RC0603FR-07523RL </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RC0603FR-076K19L </t>
+  </si>
+  <si>
+    <t>R11,R21,R32,R38,R39,R52,R63</t>
+  </si>
+  <si>
+    <t>SMR20200325</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1245,28 +1336,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K44"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.88671875" customWidth="1"/>
-    <col min="5" max="5" width="23.44140625" customWidth="1"/>
-    <col min="8" max="8" width="59.88671875" customWidth="1"/>
-    <col min="9" max="9" width="11.33203125" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" customWidth="1"/>
+    <col min="5" max="5" width="23.42578125" customWidth="1"/>
+    <col min="8" max="8" width="59.85546875" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
         <v>116</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
         <v>59</v>
       </c>
@@ -1276,7 +1367,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>0</v>
       </c>
@@ -1311,7 +1402,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -1340,7 +1431,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -1351,7 +1442,7 @@
         <v>1</v>
       </c>
       <c r="D7">
-        <f t="shared" ref="D7:D21" si="0">C7*D$3</f>
+        <f t="shared" ref="D7:D32" si="0">C7*D$3</f>
         <v>3</v>
       </c>
       <c r="E7" t="s">
@@ -1369,7 +1460,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -1398,7 +1489,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -1421,7 +1512,7 @@
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -1450,7 +1541,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -1473,7 +1564,7 @@
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -1496,7 +1587,7 @@
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -1519,7 +1610,913 @@
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>120</v>
+      </c>
+      <c r="B14" t="s">
+        <v>121</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E14" t="s">
+        <v>122</v>
+      </c>
+      <c r="G14" t="s">
+        <v>123</v>
+      </c>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>52</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E15" t="s">
+        <v>54</v>
+      </c>
+      <c r="F15" t="s">
+        <v>55</v>
+      </c>
+      <c r="G15" t="s">
+        <v>56</v>
+      </c>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>135</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C16">
+        <v>2</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="E16" t="s">
+        <v>14</v>
+      </c>
+      <c r="F16" t="s">
+        <v>58</v>
+      </c>
+      <c r="G16" t="s">
+        <v>22</v>
+      </c>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>79</v>
+      </c>
+      <c r="B17" t="s">
+        <v>109</v>
+      </c>
+      <c r="C17">
+        <v>10</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="E17" t="s">
+        <v>20</v>
+      </c>
+      <c r="F17" t="s">
+        <v>21</v>
+      </c>
+      <c r="G17" t="s">
+        <v>22</v>
+      </c>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>80</v>
+      </c>
+      <c r="B18" t="s">
+        <v>110</v>
+      </c>
+      <c r="C18">
+        <v>4</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="E18" t="s">
+        <v>14</v>
+      </c>
+      <c r="F18" t="s">
+        <v>31</v>
+      </c>
+      <c r="G18" t="s">
+        <v>22</v>
+      </c>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>124</v>
+      </c>
+      <c r="B19" t="s">
+        <v>126</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E19" t="s">
+        <v>14</v>
+      </c>
+      <c r="F19" t="s">
+        <v>128</v>
+      </c>
+      <c r="G19" t="s">
+        <v>22</v>
+      </c>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>125</v>
+      </c>
+      <c r="B20" t="s">
+        <v>127</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E20" t="s">
+        <v>20</v>
+      </c>
+      <c r="F20" t="s">
+        <v>129</v>
+      </c>
+      <c r="G20" t="s">
+        <v>22</v>
+      </c>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>131</v>
+      </c>
+      <c r="B21" t="s">
+        <v>132</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E21" t="s">
+        <v>14</v>
+      </c>
+      <c r="F21" t="s">
+        <v>133</v>
+      </c>
+      <c r="G21" t="s">
+        <v>13</v>
+      </c>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>61</v>
+      </c>
+      <c r="B22" t="s">
+        <v>23</v>
+      </c>
+      <c r="C22">
+        <v>2</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="E22" t="s">
+        <v>24</v>
+      </c>
+      <c r="G22" t="s">
+        <v>22</v>
+      </c>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>148</v>
+      </c>
+      <c r="B23" t="s">
+        <v>28</v>
+      </c>
+      <c r="C23">
+        <v>7</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="E23" t="s">
+        <v>25</v>
+      </c>
+      <c r="F23" t="s">
+        <v>26</v>
+      </c>
+      <c r="G23" t="s">
+        <v>22</v>
+      </c>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>66</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C24">
+        <v>2</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="E24" t="s">
+        <v>25</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="G24" t="s">
+        <v>22</v>
+      </c>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>134</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C25">
+        <v>2</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="E25" t="s">
+        <v>25</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G25" t="s">
+        <v>22</v>
+      </c>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>30</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E26" t="s">
+        <v>25</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="G26" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>112</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C27">
+        <v>3</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="E27" t="s">
+        <v>25</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G27" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>113</v>
+      </c>
+      <c r="B28" s="2"/>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E28" t="s">
+        <v>114</v>
+      </c>
+      <c r="F28" s="3"/>
+      <c r="G28" t="s">
+        <v>13</v>
+      </c>
+      <c r="H28" t="s">
+        <v>115</v>
+      </c>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>136</v>
+      </c>
+      <c r="B29" t="s">
+        <v>140</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E29" t="s">
+        <v>25</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="G29" t="s">
+        <v>22</v>
+      </c>
+      <c r="I29" s="1"/>
+      <c r="J29" s="1"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>137</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E30" t="s">
+        <v>25</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="G30" t="s">
+        <v>22</v>
+      </c>
+      <c r="I30" s="1"/>
+      <c r="J30" s="1"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>138</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
+      <c r="D31">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E31" t="s">
+        <v>25</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="G31" t="s">
+        <v>22</v>
+      </c>
+      <c r="I31" s="1"/>
+      <c r="J31" s="1"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>143</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="D32">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E32" t="s">
+        <v>25</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="G32" t="s">
+        <v>22</v>
+      </c>
+      <c r="I32" s="1"/>
+      <c r="J32" s="1"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I33" s="1"/>
+      <c r="J33" s="1"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>96</v>
+      </c>
+      <c r="B35" t="s">
+        <v>97</v>
+      </c>
+      <c r="C35">
+        <v>1</v>
+      </c>
+      <c r="D35">
+        <f>C35*D$3</f>
+        <v>3</v>
+      </c>
+      <c r="E35" t="s">
+        <v>98</v>
+      </c>
+      <c r="F35" t="s">
+        <v>99</v>
+      </c>
+      <c r="I35" s="1"/>
+      <c r="J35" s="1"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="B36" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="C36">
+        <v>1</v>
+      </c>
+      <c r="D36">
+        <f>C36*D$3</f>
+        <v>3</v>
+      </c>
+      <c r="E36" t="s">
+        <v>103</v>
+      </c>
+      <c r="I36" s="1"/>
+      <c r="J36" s="1"/>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" s="18"/>
+      <c r="B37" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C37">
+        <v>1</v>
+      </c>
+      <c r="D37">
+        <f>C37*D$3</f>
+        <v>3</v>
+      </c>
+      <c r="E37" t="s">
+        <v>106</v>
+      </c>
+      <c r="I37" s="1"/>
+      <c r="J37" s="1"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38" s="18"/>
+      <c r="B38" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C38">
+        <v>2</v>
+      </c>
+      <c r="D38">
+        <f>C38*D$3</f>
+        <v>6</v>
+      </c>
+      <c r="E38" t="s">
+        <v>107</v>
+      </c>
+      <c r="F38" s="3"/>
+      <c r="I38" s="1"/>
+      <c r="J38" s="1"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B39" s="2"/>
+      <c r="I39" s="1"/>
+      <c r="J39" s="1"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F40" s="3"/>
+      <c r="I40" s="1"/>
+      <c r="J40" s="1"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F41" s="3"/>
+      <c r="I41" s="1"/>
+      <c r="J41" s="1"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F42" s="3"/>
+      <c r="I42" s="1"/>
+      <c r="J42" s="1"/>
+    </row>
+    <row r="43" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F43" s="8"/>
+      <c r="H43" s="6"/>
+      <c r="I43" s="9"/>
+      <c r="J43" s="10"/>
+    </row>
+    <row r="44" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="11"/>
+      <c r="F44" s="8"/>
+      <c r="H44" s="6"/>
+      <c r="I44" s="9"/>
+      <c r="J44" s="10"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F45" s="3"/>
+      <c r="H45" s="2"/>
+      <c r="I45" s="4"/>
+      <c r="J45" s="1"/>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I47" s="1"/>
+      <c r="J47" s="1"/>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B48" s="1"/>
+    </row>
+    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B49" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A36:A38"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K44"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="17.85546875" customWidth="1"/>
+    <col min="5" max="5" width="23.42578125" customWidth="1"/>
+    <col min="8" max="8" width="59.85546875" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <f>C6*D$3</f>
+        <v>3</v>
+      </c>
+      <c r="E6" t="s">
+        <v>33</v>
+      </c>
+      <c r="G6" t="s">
+        <v>34</v>
+      </c>
+      <c r="H6" t="s">
+        <v>36</v>
+      </c>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <f t="shared" ref="D7:D21" si="0">C7*D$3</f>
+        <v>3</v>
+      </c>
+      <c r="E7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G7" t="s">
+        <v>34</v>
+      </c>
+      <c r="H7" t="s">
+        <v>38</v>
+      </c>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E8" t="s">
+        <v>40</v>
+      </c>
+      <c r="G8" t="s">
+        <v>41</v>
+      </c>
+      <c r="H8" t="s">
+        <v>42</v>
+      </c>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
+        <v>90</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E9" t="s">
+        <v>47</v>
+      </c>
+      <c r="G9" t="s">
+        <v>94</v>
+      </c>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E10" t="s">
+        <v>44</v>
+      </c>
+      <c r="G10" t="s">
+        <v>45</v>
+      </c>
+      <c r="H10" t="s">
+        <v>46</v>
+      </c>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="14" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" t="s">
+        <v>76</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E11" t="s">
+        <v>77</v>
+      </c>
+      <c r="G11" t="s">
+        <v>78</v>
+      </c>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E12" t="s">
+        <v>51</v>
+      </c>
+      <c r="G12" t="s">
+        <v>19</v>
+      </c>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" t="s">
+        <v>49</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E13" t="s">
+        <v>50</v>
+      </c>
+      <c r="G13" t="s">
+        <v>19</v>
+      </c>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>62</v>
       </c>
@@ -1542,7 +2539,7 @@
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>52</v>
       </c>
@@ -1568,7 +2565,7 @@
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>57</v>
       </c>
@@ -1594,7 +2591,7 @@
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>79</v>
       </c>
@@ -1620,7 +2617,7 @@
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>80</v>
       </c>
@@ -1646,7 +2643,7 @@
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>61</v>
       </c>
@@ -1669,7 +2666,7 @@
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>91</v>
       </c>
@@ -1695,7 +2692,7 @@
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>66</v>
       </c>
@@ -1721,7 +2718,7 @@
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>92</v>
       </c>
@@ -1747,7 +2744,7 @@
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>81</v>
       </c>
@@ -1773,7 +2770,7 @@
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>93</v>
       </c>
@@ -1797,7 +2794,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>30</v>
       </c>
@@ -1821,7 +2818,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>112</v>
       </c>
@@ -1845,7 +2842,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>113</v>
       </c>
@@ -1870,16 +2867,16 @@
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>96</v>
       </c>
@@ -1902,7 +2899,7 @@
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="18" t="s">
         <v>101</v>
       </c>
@@ -1922,7 +2919,7 @@
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="18"/>
       <c r="B32" s="3" t="s">
         <v>104</v>
@@ -1940,7 +2937,7 @@
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="18"/>
       <c r="B33" s="2" t="s">
         <v>105</v>
@@ -1959,53 +2956,53 @@
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B34" s="2"/>
       <c r="I34" s="1"/>
       <c r="J34" s="1"/>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F35" s="3"/>
       <c r="I35" s="1"/>
       <c r="J35" s="1"/>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F36" s="3"/>
       <c r="I36" s="1"/>
       <c r="J36" s="1"/>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F37" s="3"/>
       <c r="I37" s="1"/>
       <c r="J37" s="1"/>
     </row>
-    <row r="38" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F38" s="8"/>
       <c r="H38" s="6"/>
       <c r="I38" s="9"/>
       <c r="J38" s="10"/>
     </row>
-    <row r="39" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B39" s="11"/>
       <c r="F39" s="8"/>
       <c r="H39" s="6"/>
       <c r="I39" s="9"/>
       <c r="J39" s="10"/>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F40" s="3"/>
       <c r="H40" s="2"/>
       <c r="I40" s="4"/>
       <c r="J40" s="1"/>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I42" s="1"/>
       <c r="J42" s="1"/>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B43" s="1"/>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B44" s="1"/>
     </row>
   </sheetData>
@@ -2018,21 +3015,21 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K43"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.88671875" customWidth="1"/>
-    <col min="5" max="5" width="23.44140625" customWidth="1"/>
-    <col min="8" max="8" width="59.88671875" customWidth="1"/>
-    <col min="9" max="9" width="11.33203125" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" customWidth="1"/>
+    <col min="5" max="5" width="23.42578125" customWidth="1"/>
+    <col min="8" max="8" width="59.85546875" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
         <v>116</v>
       </c>
@@ -2043,7 +3040,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
         <v>59</v>
       </c>
@@ -2053,7 +3050,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>0</v>
       </c>
@@ -2088,7 +3085,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -2117,7 +3114,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -2146,7 +3143,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -2175,7 +3172,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -2198,7 +3195,7 @@
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -2227,7 +3224,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -2250,7 +3247,7 @@
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -2273,7 +3270,7 @@
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -2296,7 +3293,7 @@
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>62</v>
       </c>
@@ -2319,7 +3316,7 @@
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>52</v>
       </c>
@@ -2345,7 +3342,7 @@
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>57</v>
       </c>
@@ -2371,7 +3368,7 @@
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>79</v>
       </c>
@@ -2397,7 +3394,7 @@
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>80</v>
       </c>
@@ -2423,7 +3420,7 @@
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>61</v>
       </c>
@@ -2446,7 +3443,7 @@
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>91</v>
       </c>
@@ -2472,7 +3469,7 @@
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>66</v>
       </c>
@@ -2498,7 +3495,7 @@
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>92</v>
       </c>
@@ -2524,7 +3521,7 @@
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>81</v>
       </c>
@@ -2550,7 +3547,7 @@
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>93</v>
       </c>
@@ -2574,7 +3571,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>30</v>
       </c>
@@ -2598,7 +3595,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>85</v>
       </c>
@@ -2627,16 +3624,16 @@
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>96</v>
       </c>
@@ -2659,7 +3656,7 @@
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="18" t="s">
         <v>101</v>
       </c>
@@ -2679,7 +3676,7 @@
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="18"/>
       <c r="B31" s="3" t="s">
         <v>104</v>
@@ -2697,7 +3694,7 @@
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="18"/>
       <c r="B32" s="2" t="s">
         <v>105</v>
@@ -2716,53 +3713,53 @@
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
     </row>
-    <row r="33" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B33" s="2"/>
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
     </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
       <c r="F34" s="3"/>
       <c r="I34" s="1"/>
       <c r="J34" s="1"/>
     </row>
-    <row r="35" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
       <c r="F35" s="3"/>
       <c r="I35" s="1"/>
       <c r="J35" s="1"/>
     </row>
-    <row r="36" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:10" x14ac:dyDescent="0.25">
       <c r="F36" s="3"/>
       <c r="I36" s="1"/>
       <c r="J36" s="1"/>
     </row>
-    <row r="37" spans="2:10" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F37" s="8"/>
       <c r="H37" s="6"/>
       <c r="I37" s="9"/>
       <c r="J37" s="10"/>
     </row>
-    <row r="38" spans="2:10" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B38" s="11"/>
       <c r="F38" s="8"/>
       <c r="H38" s="6"/>
       <c r="I38" s="9"/>
       <c r="J38" s="10"/>
     </row>
-    <row r="39" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:10" x14ac:dyDescent="0.25">
       <c r="F39" s="3"/>
       <c r="H39" s="2"/>
       <c r="I39" s="4"/>
       <c r="J39" s="1"/>
     </row>
-    <row r="41" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:10" x14ac:dyDescent="0.25">
       <c r="I41" s="1"/>
       <c r="J41" s="1"/>
     </row>
-    <row r="42" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B42" s="1"/>
     </row>
-    <row r="43" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B43" s="1"/>
     </row>
   </sheetData>

</xml_diff>